<commit_message>
Upload Y4_B2526_General_Surgery_checklist1758703665957_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_checklist1758703665957_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_checklist1758703665957_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94314453-DC6A-43B9-8780-A4A92A77AE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C50B40-14E2-4320-B69C-71D598A0E73C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="1300" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Surgery" sheetId="1" r:id="rId1"/>
@@ -473,10 +473,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -505,7 +512,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -847,16 +854,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="10.25" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -876,7 +883,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -887,7 +894,7 @@
         <v>45916</v>
       </c>
       <c r="D2" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.46059027777777778</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -896,7 +903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -907,7 +914,7 @@
         <v>45916</v>
       </c>
       <c r="D3" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.46059027777777778</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -916,7 +923,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -927,7 +934,7 @@
         <v>45916</v>
       </c>
       <c r="D4" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -936,7 +943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -947,7 +954,7 @@
         <v>45916</v>
       </c>
       <c r="D5" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -956,7 +963,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -967,7 +974,7 @@
         <v>45916</v>
       </c>
       <c r="D6" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -976,7 +983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -987,7 +994,7 @@
         <v>45916</v>
       </c>
       <c r="D7" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -996,7 +1003,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1007,7 +1014,7 @@
         <v>45916</v>
       </c>
       <c r="D8" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -1016,7 +1023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1027,7 +1034,7 @@
         <v>45916</v>
       </c>
       <c r="D9" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -1036,7 +1043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1047,7 +1054,7 @@
         <v>45916</v>
       </c>
       <c r="D10" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -1056,7 +1063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1067,7 +1074,7 @@
         <v>45916</v>
       </c>
       <c r="D11" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -1076,7 +1083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1087,7 +1094,7 @@
         <v>45916</v>
       </c>
       <c r="D12" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
@@ -1096,7 +1103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1107,7 +1114,7 @@
         <v>45916</v>
       </c>
       <c r="D13" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
@@ -1116,7 +1123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1127,7 +1134,7 @@
         <v>45916</v>
       </c>
       <c r="D14" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -1136,7 +1143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1147,7 +1154,7 @@
         <v>45916</v>
       </c>
       <c r="D15" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -1156,7 +1163,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1167,7 +1174,7 @@
         <v>45916</v>
       </c>
       <c r="D16" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
@@ -1176,7 +1183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1187,7 +1194,7 @@
         <v>45916</v>
       </c>
       <c r="D17" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
@@ -1196,7 +1203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1207,7 +1214,7 @@
         <v>45916</v>
       </c>
       <c r="D18" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
@@ -1216,7 +1223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1227,7 +1234,7 @@
         <v>45916</v>
       </c>
       <c r="D19" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -1236,7 +1243,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1247,7 +1254,7 @@
         <v>45916</v>
       </c>
       <c r="D20" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E20" t="s">
         <v>8</v>
@@ -1256,7 +1263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1267,7 +1274,7 @@
         <v>45916</v>
       </c>
       <c r="D21" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
@@ -1276,7 +1283,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1287,7 +1294,7 @@
         <v>45916</v>
       </c>
       <c r="D22" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
@@ -1296,7 +1303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1307,7 +1314,7 @@
         <v>45916</v>
       </c>
       <c r="D23" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
@@ -1316,7 +1323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1327,7 +1334,7 @@
         <v>45916</v>
       </c>
       <c r="D24" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
@@ -1336,7 +1343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1347,7 +1354,7 @@
         <v>45916</v>
       </c>
       <c r="D25" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E25" t="s">
         <v>8</v>
@@ -1356,7 +1363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1367,7 +1374,7 @@
         <v>45916</v>
       </c>
       <c r="D26" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E26" t="s">
         <v>8</v>
@@ -1376,7 +1383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1387,7 +1394,7 @@
         <v>45916</v>
       </c>
       <c r="D27" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E27" t="s">
         <v>8</v>
@@ -1396,7 +1403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -1407,7 +1414,7 @@
         <v>45916</v>
       </c>
       <c r="D28" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E28" t="s">
         <v>8</v>
@@ -1416,7 +1423,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -1427,7 +1434,7 @@
         <v>45916</v>
       </c>
       <c r="D29" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E29" t="s">
         <v>8</v>
@@ -1436,7 +1443,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -1447,7 +1454,7 @@
         <v>45916</v>
       </c>
       <c r="D30" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E30" t="s">
         <v>8</v>
@@ -1456,7 +1463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -1467,7 +1474,7 @@
         <v>45916</v>
       </c>
       <c r="D31" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E31" t="s">
         <v>8</v>
@@ -1476,7 +1483,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -1487,7 +1494,7 @@
         <v>45916</v>
       </c>
       <c r="D32" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E32" t="s">
         <v>8</v>
@@ -1496,7 +1503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -1507,7 +1514,7 @@
         <v>45916</v>
       </c>
       <c r="D33" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E33" t="s">
         <v>8</v>
@@ -1516,7 +1523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -1527,7 +1534,7 @@
         <v>45916</v>
       </c>
       <c r="D34" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E34" t="s">
         <v>8</v>
@@ -1536,7 +1543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -1547,7 +1554,7 @@
         <v>45916</v>
       </c>
       <c r="D35" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E35" t="s">
         <v>8</v>
@@ -1556,7 +1563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -1567,7 +1574,7 @@
         <v>45916</v>
       </c>
       <c r="D36" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E36" t="s">
         <v>8</v>
@@ -1576,7 +1583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -1587,7 +1594,7 @@
         <v>45916</v>
       </c>
       <c r="D37" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E37" t="s">
         <v>8</v>
@@ -1596,7 +1603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -1607,7 +1614,7 @@
         <v>45916</v>
       </c>
       <c r="D38" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E38" t="s">
         <v>8</v>
@@ -1616,7 +1623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -1627,7 +1634,7 @@
         <v>45916</v>
       </c>
       <c r="D39" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E39" t="s">
         <v>8</v>
@@ -1636,7 +1643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -1647,7 +1654,7 @@
         <v>45916</v>
       </c>
       <c r="D40" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E40" t="s">
         <v>8</v>
@@ -1656,7 +1663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -1667,7 +1674,7 @@
         <v>45916</v>
       </c>
       <c r="D41" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E41" t="s">
         <v>8</v>
@@ -1676,7 +1683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -1687,7 +1694,7 @@
         <v>45916</v>
       </c>
       <c r="D42" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E42" t="s">
         <v>8</v>
@@ -1696,7 +1703,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>50</v>
       </c>
@@ -1707,7 +1714,7 @@
         <v>45916</v>
       </c>
       <c r="D43" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E43" t="s">
         <v>8</v>
@@ -1716,7 +1723,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -1727,7 +1734,7 @@
         <v>45916</v>
       </c>
       <c r="D44" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E44" t="s">
         <v>8</v>
@@ -1736,7 +1743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -1747,7 +1754,7 @@
         <v>45916</v>
       </c>
       <c r="D45" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E45" t="s">
         <v>8</v>
@@ -1756,7 +1763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>53</v>
       </c>
@@ -1767,7 +1774,7 @@
         <v>45916</v>
       </c>
       <c r="D46" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E46" t="s">
         <v>8</v>
@@ -1776,7 +1783,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>54</v>
       </c>
@@ -1787,7 +1794,7 @@
         <v>45916</v>
       </c>
       <c r="D47" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E47" t="s">
         <v>8</v>
@@ -1796,7 +1803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -1807,7 +1814,7 @@
         <v>45916</v>
       </c>
       <c r="D48" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E48" t="s">
         <v>8</v>
@@ -1816,7 +1823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -1827,7 +1834,7 @@
         <v>45916</v>
       </c>
       <c r="D49" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E49" t="s">
         <v>8</v>
@@ -1836,7 +1843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -1847,7 +1854,7 @@
         <v>45916</v>
       </c>
       <c r="D50" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E50" t="s">
         <v>8</v>
@@ -1856,7 +1863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -1867,7 +1874,7 @@
         <v>45916</v>
       </c>
       <c r="D51" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E51" t="s">
         <v>8</v>
@@ -1876,7 +1883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -1887,7 +1894,7 @@
         <v>45916</v>
       </c>
       <c r="D52" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E52" t="s">
         <v>8</v>
@@ -1896,7 +1903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -1907,7 +1914,7 @@
         <v>45916</v>
       </c>
       <c r="D53" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E53" t="s">
         <v>8</v>
@@ -1916,7 +1923,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>61</v>
       </c>
@@ -1927,7 +1934,7 @@
         <v>45916</v>
       </c>
       <c r="D54" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E54" t="s">
         <v>8</v>
@@ -1936,7 +1943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>62</v>
       </c>
@@ -1947,7 +1954,7 @@
         <v>45916</v>
       </c>
       <c r="D55" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E55" t="s">
         <v>8</v>
@@ -1956,7 +1963,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -1967,7 +1974,7 @@
         <v>45916</v>
       </c>
       <c r="D56" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E56" t="s">
         <v>8</v>
@@ -1976,7 +1983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>64</v>
       </c>
@@ -1987,7 +1994,7 @@
         <v>45916</v>
       </c>
       <c r="D57" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E57" t="s">
         <v>8</v>
@@ -1996,7 +2003,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>65</v>
       </c>
@@ -2007,7 +2014,7 @@
         <v>45916</v>
       </c>
       <c r="D58" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E58" t="s">
         <v>8</v>
@@ -2016,7 +2023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>66</v>
       </c>
@@ -2027,7 +2034,7 @@
         <v>45916</v>
       </c>
       <c r="D59" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E59" t="s">
         <v>8</v>
@@ -2036,7 +2043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>67</v>
       </c>
@@ -2047,7 +2054,7 @@
         <v>45916</v>
       </c>
       <c r="D60" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E60" t="s">
         <v>8</v>
@@ -2056,7 +2063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -2067,7 +2074,7 @@
         <v>45916</v>
       </c>
       <c r="D61" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E61" t="s">
         <v>8</v>
@@ -2076,7 +2083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>69</v>
       </c>
@@ -2087,7 +2094,7 @@
         <v>45916</v>
       </c>
       <c r="D62" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E62" t="s">
         <v>8</v>
@@ -2096,7 +2103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>70</v>
       </c>
@@ -2107,7 +2114,7 @@
         <v>45916</v>
       </c>
       <c r="D63" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E63" t="s">
         <v>8</v>
@@ -2116,7 +2123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>71</v>
       </c>
@@ -2127,7 +2134,7 @@
         <v>45916</v>
       </c>
       <c r="D64" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E64" t="s">
         <v>8</v>
@@ -2136,7 +2143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>72</v>
       </c>
@@ -2147,7 +2154,7 @@
         <v>45916</v>
       </c>
       <c r="D65" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E65" t="s">
         <v>8</v>
@@ -2156,7 +2163,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>73</v>
       </c>
@@ -2167,7 +2174,7 @@
         <v>45916</v>
       </c>
       <c r="D66" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E66" t="s">
         <v>8</v>
@@ -2176,7 +2183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -2187,7 +2194,7 @@
         <v>45916</v>
       </c>
       <c r="D67" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E67" t="s">
         <v>8</v>
@@ -2196,7 +2203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -2207,7 +2214,7 @@
         <v>45916</v>
       </c>
       <c r="D68" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E68" t="s">
         <v>8</v>
@@ -2216,7 +2223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -2227,7 +2234,7 @@
         <v>45916</v>
       </c>
       <c r="D69" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E69" t="s">
         <v>8</v>
@@ -2236,7 +2243,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -2247,7 +2254,7 @@
         <v>45916</v>
       </c>
       <c r="D70" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E70" t="s">
         <v>8</v>
@@ -2256,7 +2263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>78</v>
       </c>
@@ -2267,7 +2274,7 @@
         <v>45916</v>
       </c>
       <c r="D71" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E71" t="s">
         <v>8</v>
@@ -2276,7 +2283,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>79</v>
       </c>
@@ -2287,7 +2294,7 @@
         <v>45916</v>
       </c>
       <c r="D72" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E72" t="s">
         <v>8</v>
@@ -2296,7 +2303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>80</v>
       </c>
@@ -2307,7 +2314,7 @@
         <v>45916</v>
       </c>
       <c r="D73" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E73" t="s">
         <v>8</v>
@@ -2316,7 +2323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>81</v>
       </c>
@@ -2327,7 +2334,7 @@
         <v>45916</v>
       </c>
       <c r="D74" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E74" t="s">
         <v>8</v>
@@ -2336,7 +2343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>82</v>
       </c>
@@ -2347,7 +2354,7 @@
         <v>45916</v>
       </c>
       <c r="D75" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E75" t="s">
         <v>8</v>
@@ -2356,7 +2363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>83</v>
       </c>
@@ -2367,7 +2374,7 @@
         <v>45916</v>
       </c>
       <c r="D76" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E76" t="s">
         <v>8</v>
@@ -2376,7 +2383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>84</v>
       </c>
@@ -2387,7 +2394,7 @@
         <v>45916</v>
       </c>
       <c r="D77" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E77" t="s">
         <v>8</v>
@@ -2396,7 +2403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>85</v>
       </c>
@@ -2407,7 +2414,7 @@
         <v>45916</v>
       </c>
       <c r="D78" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E78" t="s">
         <v>8</v>
@@ -2416,7 +2423,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>86</v>
       </c>
@@ -2427,7 +2434,7 @@
         <v>45916</v>
       </c>
       <c r="D79" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E79" t="s">
         <v>8</v>
@@ -2436,7 +2443,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>87</v>
       </c>
@@ -2447,7 +2454,7 @@
         <v>45916</v>
       </c>
       <c r="D80" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E80" t="s">
         <v>8</v>
@@ -2456,7 +2463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>88</v>
       </c>
@@ -2467,7 +2474,7 @@
         <v>45916</v>
       </c>
       <c r="D81" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E81" t="s">
         <v>8</v>
@@ -2476,7 +2483,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>89</v>
       </c>
@@ -2487,7 +2494,7 @@
         <v>45916</v>
       </c>
       <c r="D82" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E82" t="s">
         <v>8</v>
@@ -2496,7 +2503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>90</v>
       </c>
@@ -2507,7 +2514,7 @@
         <v>45916</v>
       </c>
       <c r="D83" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E83" t="s">
         <v>8</v>
@@ -2516,7 +2523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>91</v>
       </c>
@@ -2527,7 +2534,7 @@
         <v>45916</v>
       </c>
       <c r="D84" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
@@ -2536,7 +2543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>92</v>
       </c>
@@ -2547,7 +2554,7 @@
         <v>45916</v>
       </c>
       <c r="D85" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E85" t="s">
         <v>8</v>
@@ -2556,7 +2563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>93</v>
       </c>
@@ -2567,7 +2574,7 @@
         <v>45916</v>
       </c>
       <c r="D86" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E86" t="s">
         <v>8</v>
@@ -2576,7 +2583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>94</v>
       </c>
@@ -2587,7 +2594,7 @@
         <v>45916</v>
       </c>
       <c r="D87" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E87" t="s">
         <v>8</v>
@@ -2596,7 +2603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>95</v>
       </c>
@@ -2607,7 +2614,7 @@
         <v>45916</v>
       </c>
       <c r="D88" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E88" t="s">
         <v>8</v>
@@ -2616,7 +2623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>96</v>
       </c>
@@ -2627,7 +2634,7 @@
         <v>45916</v>
       </c>
       <c r="D89" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E89" t="s">
         <v>8</v>
@@ -2636,7 +2643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>97</v>
       </c>
@@ -2647,7 +2654,7 @@
         <v>45916</v>
       </c>
       <c r="D90" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E90" t="s">
         <v>8</v>
@@ -2656,7 +2663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>98</v>
       </c>
@@ -2667,7 +2674,7 @@
         <v>45916</v>
       </c>
       <c r="D91" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E91" t="s">
         <v>8</v>
@@ -2676,7 +2683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>99</v>
       </c>
@@ -2687,7 +2694,7 @@
         <v>45916</v>
       </c>
       <c r="D92" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E92" t="s">
         <v>8</v>
@@ -2696,7 +2703,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>100</v>
       </c>
@@ -2707,7 +2714,7 @@
         <v>45916</v>
       </c>
       <c r="D93" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E93" t="s">
         <v>8</v>
@@ -2716,7 +2723,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>101</v>
       </c>
@@ -2727,7 +2734,7 @@
         <v>45916</v>
       </c>
       <c r="D94" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E94" t="s">
         <v>8</v>
@@ -2736,7 +2743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>102</v>
       </c>
@@ -2747,7 +2754,7 @@
         <v>45916</v>
       </c>
       <c r="D95" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E95" t="s">
         <v>8</v>
@@ -2756,7 +2763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>103</v>
       </c>
@@ -2767,7 +2774,7 @@
         <v>45916</v>
       </c>
       <c r="D96" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E96" t="s">
         <v>8</v>
@@ -2776,7 +2783,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>104</v>
       </c>
@@ -2787,7 +2794,7 @@
         <v>45916</v>
       </c>
       <c r="D97" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E97" t="s">
         <v>8</v>
@@ -2796,7 +2803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>105</v>
       </c>
@@ -2807,7 +2814,7 @@
         <v>45916</v>
       </c>
       <c r="D98" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E98" t="s">
         <v>8</v>
@@ -2816,7 +2823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>106</v>
       </c>
@@ -2827,7 +2834,7 @@
         <v>45916</v>
       </c>
       <c r="D99" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E99" t="s">
         <v>8</v>
@@ -2836,7 +2843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>107</v>
       </c>
@@ -2847,7 +2854,7 @@
         <v>45916</v>
       </c>
       <c r="D100" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E100" t="s">
         <v>8</v>
@@ -2856,7 +2863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>108</v>
       </c>
@@ -2867,7 +2874,7 @@
         <v>45916</v>
       </c>
       <c r="D101" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E101" t="s">
         <v>8</v>
@@ -2876,7 +2883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>109</v>
       </c>
@@ -2887,7 +2894,7 @@
         <v>45916</v>
       </c>
       <c r="D102" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E102" t="s">
         <v>8</v>
@@ -2896,7 +2903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>110</v>
       </c>
@@ -2907,7 +2914,7 @@
         <v>45916</v>
       </c>
       <c r="D103" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E103" t="s">
         <v>8</v>
@@ -2916,7 +2923,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>111</v>
       </c>
@@ -2927,7 +2934,7 @@
         <v>45916</v>
       </c>
       <c r="D104" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E104" t="s">
         <v>8</v>
@@ -2936,7 +2943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>112</v>
       </c>
@@ -2947,7 +2954,7 @@
         <v>45916</v>
       </c>
       <c r="D105" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E105" t="s">
         <v>8</v>
@@ -2956,7 +2963,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>113</v>
       </c>
@@ -2967,7 +2974,7 @@
         <v>45916</v>
       </c>
       <c r="D106" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E106" t="s">
         <v>8</v>
@@ -2976,7 +2983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>114</v>
       </c>
@@ -2987,7 +2994,7 @@
         <v>45916</v>
       </c>
       <c r="D107" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E107" t="s">
         <v>8</v>
@@ -2996,7 +3003,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>115</v>
       </c>
@@ -3007,7 +3014,7 @@
         <v>45916</v>
       </c>
       <c r="D108" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E108" t="s">
         <v>8</v>
@@ -3016,7 +3023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>116</v>
       </c>
@@ -3027,7 +3034,7 @@
         <v>45916</v>
       </c>
       <c r="D109" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E109" t="s">
         <v>8</v>
@@ -3036,7 +3043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>117</v>
       </c>
@@ -3047,7 +3054,7 @@
         <v>45916</v>
       </c>
       <c r="D110" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E110" t="s">
         <v>8</v>
@@ -3056,7 +3063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>118</v>
       </c>
@@ -3067,7 +3074,7 @@
         <v>45916</v>
       </c>
       <c r="D111" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E111" t="s">
         <v>8</v>
@@ -3076,7 +3083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>119</v>
       </c>
@@ -3087,7 +3094,7 @@
         <v>45916</v>
       </c>
       <c r="D112" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E112" t="s">
         <v>8</v>
@@ -3096,7 +3103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>120</v>
       </c>
@@ -3107,7 +3114,7 @@
         <v>45916</v>
       </c>
       <c r="D113" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E113" t="s">
         <v>8</v>
@@ -3116,7 +3123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>121</v>
       </c>
@@ -3127,7 +3134,7 @@
         <v>45916</v>
       </c>
       <c r="D114" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E114" t="s">
         <v>8</v>
@@ -3136,7 +3143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>122</v>
       </c>
@@ -3147,7 +3154,7 @@
         <v>45916</v>
       </c>
       <c r="D115" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E115" t="s">
         <v>8</v>
@@ -3156,7 +3163,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>123</v>
       </c>
@@ -3167,7 +3174,7 @@
         <v>45916</v>
       </c>
       <c r="D116" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E116" t="s">
         <v>8</v>
@@ -3176,7 +3183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>124</v>
       </c>
@@ -3187,7 +3194,7 @@
         <v>45916</v>
       </c>
       <c r="D117" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E117" t="s">
         <v>8</v>
@@ -3196,7 +3203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>125</v>
       </c>
@@ -3207,7 +3214,7 @@
         <v>45916</v>
       </c>
       <c r="D118" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E118" t="s">
         <v>8</v>
@@ -3216,7 +3223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>126</v>
       </c>
@@ -3227,7 +3234,7 @@
         <v>45916</v>
       </c>
       <c r="D119" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E119" t="s">
         <v>8</v>
@@ -3236,7 +3243,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>127</v>
       </c>
@@ -3247,7 +3254,7 @@
         <v>45916</v>
       </c>
       <c r="D120" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E120" t="s">
         <v>8</v>
@@ -3256,7 +3263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>128</v>
       </c>
@@ -3267,7 +3274,7 @@
         <v>45916</v>
       </c>
       <c r="D121" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E121" t="s">
         <v>8</v>
@@ -3276,7 +3283,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>129</v>
       </c>
@@ -3287,7 +3294,7 @@
         <v>45916</v>
       </c>
       <c r="D122" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E122" t="s">
         <v>8</v>
@@ -3296,7 +3303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>130</v>
       </c>
@@ -3307,7 +3314,7 @@
         <v>45916</v>
       </c>
       <c r="D123" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E123" t="s">
         <v>8</v>
@@ -3316,7 +3323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>131</v>
       </c>
@@ -3327,7 +3334,7 @@
         <v>45916</v>
       </c>
       <c r="D124" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E124" t="s">
         <v>8</v>
@@ -3336,7 +3343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>132</v>
       </c>
@@ -3347,7 +3354,7 @@
         <v>45916</v>
       </c>
       <c r="D125" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E125" t="s">
         <v>8</v>
@@ -3356,7 +3363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>133</v>
       </c>
@@ -3367,7 +3374,7 @@
         <v>45916</v>
       </c>
       <c r="D126" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E126" t="s">
         <v>8</v>
@@ -3376,7 +3383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>134</v>
       </c>
@@ -3387,7 +3394,7 @@
         <v>45916</v>
       </c>
       <c r="D127" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E127" t="s">
         <v>8</v>
@@ -3396,7 +3403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>135</v>
       </c>
@@ -3407,7 +3414,7 @@
         <v>45916</v>
       </c>
       <c r="D128" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E128" t="s">
         <v>8</v>
@@ -3416,7 +3423,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>136</v>
       </c>
@@ -3427,7 +3434,7 @@
         <v>45916</v>
       </c>
       <c r="D129" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E129" t="s">
         <v>8</v>
@@ -3436,7 +3443,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>137</v>
       </c>
@@ -3447,7 +3454,7 @@
         <v>45916</v>
       </c>
       <c r="D130" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E130" t="s">
         <v>8</v>
@@ -3456,7 +3463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>138</v>
       </c>
@@ -3467,7 +3474,7 @@
         <v>45916</v>
       </c>
       <c r="D131" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E131" t="s">
         <v>8</v>
@@ -3476,7 +3483,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>139</v>
       </c>
@@ -3487,7 +3494,7 @@
         <v>45916</v>
       </c>
       <c r="D132" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E132" t="s">
         <v>8</v>
@@ -3496,7 +3503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>140</v>
       </c>
@@ -3507,7 +3514,7 @@
         <v>45916</v>
       </c>
       <c r="D133" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E133" t="s">
         <v>8</v>
@@ -3516,7 +3523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>141</v>
       </c>
@@ -3527,7 +3534,7 @@
         <v>45916</v>
       </c>
       <c r="D134" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E134" t="s">
         <v>8</v>
@@ -3536,7 +3543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>142</v>
       </c>
@@ -3547,7 +3554,7 @@
         <v>45916</v>
       </c>
       <c r="D135" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E135" t="s">
         <v>8</v>
@@ -3556,7 +3563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>143</v>
       </c>
@@ -3567,7 +3574,7 @@
         <v>45916</v>
       </c>
       <c r="D136" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E136" t="s">
         <v>8</v>
@@ -3576,7 +3583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>144</v>
       </c>
@@ -3587,7 +3594,7 @@
         <v>45916</v>
       </c>
       <c r="D137" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E137" t="s">
         <v>8</v>
@@ -3596,7 +3603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>145</v>
       </c>
@@ -3607,7 +3614,7 @@
         <v>45916</v>
       </c>
       <c r="D138" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E138" t="s">
         <v>8</v>
@@ -3616,7 +3623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>146</v>
       </c>
@@ -3627,7 +3634,7 @@
         <v>45916</v>
       </c>
       <c r="D139" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E139" t="s">
         <v>8</v>
@@ -3636,7 +3643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>147</v>
       </c>
@@ -3647,7 +3654,7 @@
         <v>45916</v>
       </c>
       <c r="D140" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E140" t="s">
         <v>8</v>
@@ -3656,7 +3663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>148</v>
       </c>
@@ -3667,7 +3674,7 @@
         <v>45916</v>
       </c>
       <c r="D141" s="2">
-        <v>0.46942129629629631</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E141" t="s">
         <v>8</v>

</xml_diff>